<commit_message>
Corrected reference designators, added OOI bar codes where necessary
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_RS01SBPD.xlsx
+++ b/deployment/Omaha_Cal_Info_RS01SBPD.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9780" yWindow="360" windowWidth="25600" windowHeight="14440" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="9780" yWindow="360" windowWidth="25605" windowHeight="14445" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
     <sheet name="ACS-158-CC_tcarray" sheetId="5" r:id="rId5"/>
     <sheet name="ACS-158-CC_taarray" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -29,13 +34,14 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A9" authorId="0">
+    <comment ref="A10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>missing from bulk load
 	-Dan Mergens</t>
@@ -47,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="118">
   <si>
     <t>Mooring OOIBARCODE</t>
   </si>
@@ -384,6 +390,27 @@
   <si>
     <t>cannot see anything until the SBPD data is ingested on a machine</t>
   </si>
+  <si>
+    <t>RS01SBPD-DP01A-00-ENG000000</t>
+  </si>
+  <si>
+    <t>RS01SBPD-DP01A-03-FLNTUA104</t>
+  </si>
+  <si>
+    <t>RS01SBPD-DP01A-ENG-00001</t>
+  </si>
+  <si>
+    <t>RS01SBPD-DP01A-ENG-00002</t>
+  </si>
+  <si>
+    <t>OL000577</t>
+  </si>
+  <si>
+    <t>OL000578</t>
+  </si>
+  <si>
+    <t>TN-314</t>
+  </si>
 </sst>
 </file>
 
@@ -395,7 +422,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.000"/>
     <numFmt numFmtId="167" formatCode="m&quot;/&quot;d&quot;/&quot;yyyy"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -404,44 +431,59 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF999999"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF222222"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF999999"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -501,7 +543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -741,12 +783,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -762,7 +816,7 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -800,6 +854,193 @@
           <a:endParaRPr lang="en-US"/>
         </a:p>
       </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>904875</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>904875</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9515475"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>904875</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="AutoShape 1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10277475" cy="9515475"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>904875</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="AutoShape 1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10277475" cy="9515475"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -1128,25 +1369,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z20"/>
+  <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="30.5" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="7" width="11.83203125" customWidth="1"/>
-    <col min="8" max="8" width="16.1640625" customWidth="1"/>
-    <col min="9" max="9" width="18.1640625" customWidth="1"/>
-    <col min="10" max="26" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="41.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="7" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1"/>
+    <col min="10" max="26" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="27" customHeight="1">
+    <row r="1" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1198,7 +1439,7 @@
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
     </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1">
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -1254,7 +1495,7 @@
       <c r="Y2" s="11"/>
       <c r="Z2" s="11"/>
     </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1">
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>18</v>
       </c>
@@ -1298,11 +1539,11 @@
         <v>-125.38066999999999</v>
       </c>
       <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
+      <c r="P3" s="16"/>
       <c r="Q3" s="11"/>
       <c r="R3" s="11"/>
       <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
+      <c r="T3" s="16"/>
       <c r="U3" s="11"/>
       <c r="V3" s="11"/>
       <c r="W3" s="11"/>
@@ -1310,12 +1551,12 @@
       <c r="Y3" s="11"/>
       <c r="Z3" s="11"/>
     </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1">
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>23</v>
+      <c r="B4" s="22" t="s">
+        <v>112</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>24</v>
@@ -1354,11 +1595,11 @@
         <v>-125.38066999999999</v>
       </c>
       <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
+      <c r="P4" s="16"/>
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
+      <c r="T4" s="16"/>
       <c r="U4" s="3"/>
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
@@ -1366,12 +1607,12 @@
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
     </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1">
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>26</v>
+      <c r="B5" s="16" t="s">
+        <v>50</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>27</v>
@@ -1410,11 +1651,11 @@
         <v>-125.38066999999999</v>
       </c>
       <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
+      <c r="P5" s="16"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
+      <c r="T5" s="16"/>
       <c r="U5" s="3"/>
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
@@ -1422,7 +1663,7 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
     </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1">
+    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
@@ -1466,11 +1707,11 @@
         <v>-125.38066999999999</v>
       </c>
       <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
+      <c r="P6" s="16"/>
       <c r="Q6" s="11"/>
       <c r="R6" s="11"/>
       <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
+      <c r="T6" s="16"/>
       <c r="U6" s="11"/>
       <c r="V6" s="11"/>
       <c r="W6" s="11"/>
@@ -1478,7 +1719,7 @@
       <c r="Y6" s="11"/>
       <c r="Z6" s="11"/>
     </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1">
+    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -1522,11 +1763,11 @@
         <v>-125.38066999999999</v>
       </c>
       <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
+      <c r="P7" s="16"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
       <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
+      <c r="T7" s="16"/>
       <c r="U7" s="3"/>
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
@@ -1534,7 +1775,7 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
         <v>33</v>
       </c>
@@ -1580,11 +1821,11 @@
         <v>-125.3801</v>
       </c>
       <c r="O8" s="22"/>
-      <c r="P8" s="3"/>
+      <c r="P8" s="16"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
       <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
+      <c r="T8" s="16"/>
       <c r="U8" s="3"/>
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
@@ -1592,99 +1833,99 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
     </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
-      <c r="V9" s="3"/>
-      <c r="W9" s="3"/>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="3"/>
-      <c r="Z9" s="3"/>
-    </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A10" s="4" t="s">
+    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" s="29">
+        <v>1</v>
+      </c>
+      <c r="E9" s="25">
+        <v>41875</v>
+      </c>
+      <c r="F9" s="26">
+        <v>0.28819444444444398</v>
+      </c>
+      <c r="G9" s="25">
+        <v>41905</v>
+      </c>
+      <c r="H9" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" s="27">
+        <v>2903</v>
+      </c>
+      <c r="K9" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="L9" s="16"/>
+      <c r="M9" s="27">
+        <f t="shared" ref="M9" si="2">((LEFT(H9,(FIND("°",H9,1)-1)))+(MID(H9,(FIND("°",H9,1)+1),(FIND("'",H9,1))-(FIND("°",H9,1)+1))/60))*(IF(RIGHT(H9,1)="N",1,-1))</f>
+        <v>44.527316666666664</v>
+      </c>
+      <c r="N9" s="27">
+        <f t="shared" ref="N9" si="3">((LEFT(I9,(FIND("°",I9,1)-1)))+(MID(I9,(FIND("°",I9,1)+1),(FIND("'",I9,1))-(FIND("°",I9,1)+1))/60))*(IF(RIGHT(I9,1)="E",1,-1))</f>
+        <v>-125.3801</v>
+      </c>
+      <c r="O9" s="22"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="22"/>
+      <c r="U9" s="22"/>
+      <c r="V9" s="22"/>
+      <c r="W9" s="22"/>
+      <c r="X9" s="22"/>
+      <c r="Y9" s="22"/>
+      <c r="Z9" s="22"/>
+    </row>
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+    </row>
+    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="D10" s="6">
-        <v>2</v>
-      </c>
-      <c r="E10" s="7">
-        <v>42207</v>
-      </c>
-      <c r="F10" s="28">
-        <v>0.92847222222222225</v>
-      </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="J10" s="10">
-        <v>2900</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="L10" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="M10" s="12">
-        <f t="shared" ref="M10:M17" si="2">((LEFT(H10,(FIND("°",H10,1)-1)))+(MID(H10,(FIND("°",H10,1)+1),(FIND("'",H10,1))-(FIND("°",H10,1)+1))/60))*(IF(RIGHT(H10,1)="N",1,-1))</f>
-        <v>44.527574999999999</v>
-      </c>
-      <c r="N10" s="12">
-        <f t="shared" ref="N10:N17" si="3">((LEFT(I10,(FIND("°",I10,1)-1)))+(MID(I10,(FIND("°",I10,1)+1),(FIND("'",I10,1))-(FIND("°",I10,1)+1))/60))*(IF(RIGHT(I10,1)="E",1,-1))</f>
-        <v>-125.38074666666667</v>
-      </c>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="11"/>
-      <c r="U10" s="11"/>
-      <c r="V10" s="11"/>
-      <c r="W10" s="11"/>
-      <c r="X10" s="11"/>
-      <c r="Y10" s="11"/>
-      <c r="Z10" s="11"/>
-    </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A11" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="14">
-        <v>459</v>
       </c>
       <c r="D11" s="6">
         <v>2</v>
@@ -1709,18 +1950,18 @@
         <v>41</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="M11" s="29">
-        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="M11" s="12">
+        <f t="shared" ref="M11:M18" si="4">((LEFT(H11,(FIND("°",H11,1)-1)))+(MID(H11,(FIND("°",H11,1)+1),(FIND("'",H11,1))-(FIND("°",H11,1)+1))/60))*(IF(RIGHT(H11,1)="N",1,-1))</f>
         <v>44.527574999999999</v>
       </c>
-      <c r="N11" s="29">
-        <f t="shared" si="3"/>
+      <c r="N11" s="12">
+        <f t="shared" ref="N11:N18" si="5">((LEFT(I11,(FIND("°",I11,1)-1)))+(MID(I11,(FIND("°",I11,1)+1),(FIND("'",I11,1))-(FIND("°",I11,1)+1))/60))*(IF(RIGHT(I11,1)="E",1,-1))</f>
         <v>-125.38074666666667</v>
       </c>
       <c r="O11" s="11"/>
-      <c r="P11" s="11"/>
+      <c r="P11" s="16"/>
       <c r="Q11" s="11"/>
       <c r="R11" s="11"/>
       <c r="S11" s="11"/>
@@ -1732,18 +1973,18 @@
       <c r="Y11" s="11"/>
       <c r="Z11" s="11"/>
     </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1">
+    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="C12" s="14">
-        <v>158</v>
+        <v>459</v>
       </c>
       <c r="D12" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" s="7">
         <v>42207</v>
@@ -1768,15 +2009,15 @@
         <v>44</v>
       </c>
       <c r="M12" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44.527574999999999</v>
       </c>
       <c r="N12" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-125.38074666666667</v>
       </c>
       <c r="O12" s="11"/>
-      <c r="P12" s="11"/>
+      <c r="P12" s="16"/>
       <c r="Q12" s="11"/>
       <c r="R12" s="11"/>
       <c r="S12" s="11"/>
@@ -1788,18 +2029,18 @@
       <c r="Y12" s="11"/>
       <c r="Z12" s="11"/>
     </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1">
+    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C13" s="14">
-        <v>3637</v>
+        <v>158</v>
       </c>
       <c r="D13" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13" s="7">
         <v>42207</v>
@@ -1824,15 +2065,15 @@
         <v>44</v>
       </c>
       <c r="M13" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44.527574999999999</v>
       </c>
       <c r="N13" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-125.38074666666667</v>
       </c>
       <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
+      <c r="P13" s="16"/>
       <c r="Q13" s="11"/>
       <c r="R13" s="11"/>
       <c r="S13" s="11"/>
@@ -1844,15 +2085,15 @@
       <c r="Y13" s="11"/>
       <c r="Z13" s="11"/>
     </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1">
+    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>112</v>
       </c>
       <c r="C14" s="14">
-        <v>3715</v>
+        <v>3637</v>
       </c>
       <c r="D14" s="6">
         <v>2</v>
@@ -1880,15 +2121,15 @@
         <v>44</v>
       </c>
       <c r="M14" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44.527574999999999</v>
       </c>
       <c r="N14" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-125.38074666666667</v>
       </c>
       <c r="O14" s="11"/>
-      <c r="P14" s="11"/>
+      <c r="P14" s="16"/>
       <c r="Q14" s="11"/>
       <c r="R14" s="11"/>
       <c r="S14" s="11"/>
@@ -1900,15 +2141,15 @@
       <c r="Y14" s="11"/>
       <c r="Z14" s="11"/>
     </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1">
+    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>29</v>
+        <v>49</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>50</v>
       </c>
       <c r="C15" s="14">
-        <v>1215</v>
+        <v>3715</v>
       </c>
       <c r="D15" s="6">
         <v>2</v>
@@ -1936,15 +2177,15 @@
         <v>44</v>
       </c>
       <c r="M15" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44.527574999999999</v>
       </c>
       <c r="N15" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-125.38074666666667</v>
       </c>
       <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
+      <c r="P15" s="16"/>
       <c r="Q15" s="11"/>
       <c r="R15" s="11"/>
       <c r="S15" s="11"/>
@@ -1956,15 +2197,15 @@
       <c r="Y15" s="11"/>
       <c r="Z15" s="11"/>
     </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1">
+    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>53</v>
+        <v>29</v>
+      </c>
+      <c r="C16" s="14">
+        <v>1215</v>
       </c>
       <c r="D16" s="6">
         <v>2</v>
@@ -1992,15 +2233,15 @@
         <v>44</v>
       </c>
       <c r="M16" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44.527574999999999</v>
       </c>
       <c r="N16" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-125.38074666666667</v>
       </c>
       <c r="O16" s="11"/>
-      <c r="P16" s="11"/>
+      <c r="P16" s="16"/>
       <c r="Q16" s="11"/>
       <c r="R16" s="11"/>
       <c r="S16" s="11"/>
@@ -2012,15 +2253,15 @@
       <c r="Y16" s="11"/>
       <c r="Z16" s="11"/>
     </row>
-    <row r="17" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A17" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="31" t="s">
-        <v>35</v>
+    <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="D17" s="6">
         <v>2</v>
@@ -2032,29 +2273,31 @@
         <v>0.92847222222222225</v>
       </c>
       <c r="G17" s="9"/>
-      <c r="H17" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="J17" s="6">
-        <v>2901</v>
+      <c r="H17" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="J17" s="10">
+        <v>2900</v>
       </c>
       <c r="K17" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="L17" s="11"/>
+      <c r="L17" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="M17" s="29">
-        <f t="shared" si="2"/>
-        <v>44.527470000000001</v>
+        <f t="shared" si="4"/>
+        <v>44.527574999999999</v>
       </c>
       <c r="N17" s="29">
-        <f t="shared" si="3"/>
-        <v>-125.38066666666667</v>
+        <f t="shared" si="5"/>
+        <v>-125.38074666666667</v>
       </c>
       <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
+      <c r="P17" s="16"/>
       <c r="Q17" s="11"/>
       <c r="R17" s="11"/>
       <c r="S17" s="11"/>
@@ -2066,51 +2309,103 @@
       <c r="Y17" s="11"/>
       <c r="Z17" s="11"/>
     </row>
-    <row r="18" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A18" s="3"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
-      <c r="T18" s="3"/>
-      <c r="U18" s="3"/>
-      <c r="V18" s="3"/>
-      <c r="W18" s="3"/>
-      <c r="X18" s="3"/>
-      <c r="Y18" s="3"/>
-      <c r="Z18" s="3"/>
-    </row>
-    <row r="19" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A19" s="3"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
+    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="6">
+        <v>2</v>
+      </c>
+      <c r="E18" s="7">
+        <v>42207</v>
+      </c>
+      <c r="F18" s="28">
+        <v>0.92847222222222225</v>
+      </c>
+      <c r="G18" s="9"/>
+      <c r="H18" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J18" s="6">
+        <v>2901</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="L18" s="11"/>
+      <c r="M18" s="29">
+        <f t="shared" si="4"/>
+        <v>44.527470000000001</v>
+      </c>
+      <c r="N18" s="29">
+        <f t="shared" si="5"/>
+        <v>-125.38066666666667</v>
+      </c>
+      <c r="O18" s="11"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="11"/>
+      <c r="V18" s="11"/>
+      <c r="W18" s="11"/>
+      <c r="X18" s="11"/>
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="11"/>
+    </row>
+    <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" s="29">
+        <v>2</v>
+      </c>
+      <c r="E19" s="9">
+        <v>42207</v>
+      </c>
+      <c r="F19" s="28">
+        <v>0.92847222222222225</v>
+      </c>
+      <c r="G19" s="9"/>
+      <c r="H19" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J19" s="29">
+        <v>2901</v>
+      </c>
+      <c r="K19" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="L19" s="16"/>
+      <c r="M19" s="29">
+        <f t="shared" ref="M19" si="6">((LEFT(H19,(FIND("°",H19,1)-1)))+(MID(H19,(FIND("°",H19,1)+1),(FIND("'",H19,1))-(FIND("°",H19,1)+1))/60))*(IF(RIGHT(H19,1)="N",1,-1))</f>
+        <v>44.527470000000001</v>
+      </c>
+      <c r="N19" s="29">
+        <f t="shared" ref="N19" si="7">((LEFT(I19,(FIND("°",I19,1)-1)))+(MID(I19,(FIND("°",I19,1)+1),(FIND("'",I19,1))-(FIND("°",I19,1)+1))/60))*(IF(RIGHT(I19,1)="E",1,-1))</f>
+        <v>-125.38066666666667</v>
+      </c>
       <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
+      <c r="P19" s="16"/>
       <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
       <c r="S19" s="3"/>
@@ -2122,7 +2417,7 @@
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
     </row>
-    <row r="20" spans="1:26" ht="15.75" customHeight="1">
+    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="23"/>
       <c r="C20" s="3"/>
@@ -2150,6 +2445,34 @@
       <c r="Y20" s="3"/>
       <c r="Z20" s="3"/>
     </row>
+    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -2164,26 +2487,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:N63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E60" sqref="E60:E61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.5" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" customWidth="1"/>
-    <col min="3" max="4" width="14.5" customWidth="1"/>
-    <col min="5" max="5" width="19.1640625" customWidth="1"/>
+    <col min="1" max="1" width="30.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="30.5" customWidth="1"/>
-    <col min="8" max="8" width="41.83203125" customWidth="1"/>
-    <col min="9" max="9" width="36.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.25" customHeight="1">
+    <row r="1" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2212,7 +2535,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1">
+    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33"/>
       <c r="B2" s="33" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A2),"""",filter(Moorings!A:A,Moorings!B:B=left(A2,14),Moorings!D:D=D2))"),"")</f>
@@ -2235,7 +2558,7 @@
       <c r="H2" s="36"/>
       <c r="I2" s="35"/>
     </row>
-    <row r="3" spans="1:9" ht="14.25" customHeight="1">
+    <row r="3" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="37" t="s">
         <v>19</v>
       </c>
@@ -2265,8 +2588,12 @@
         <v>44.527316666666664</v>
       </c>
       <c r="I3" s="41"/>
-    </row>
-    <row r="4" spans="1:9" ht="14.25" customHeight="1">
+      <c r="N3" t="e">
+        <f t="shared" ref="N3:N9" si="0">MATCH(L3,A:A,0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="37" t="s">
         <v>19</v>
       </c>
@@ -2296,8 +2623,12 @@
         <v>-125.3801</v>
       </c>
       <c r="I4" s="41"/>
-    </row>
-    <row r="5" spans="1:9" ht="14.25" customHeight="1">
+      <c r="N4" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="41"/>
       <c r="B5" s="33" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A5),"""",filter(Moorings!A:A,Moorings!B:B=left(A5,14),Moorings!D:D=D5))"),"")</f>
@@ -2319,8 +2650,12 @@
       <c r="G5" s="41"/>
       <c r="H5" s="42"/>
       <c r="I5" s="41"/>
-    </row>
-    <row r="6" spans="1:9" ht="14.25" customHeight="1">
+      <c r="N5" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="41" t="s">
         <v>19</v>
       </c>
@@ -2350,8 +2685,12 @@
         <v>44.527316666666664</v>
       </c>
       <c r="I6" s="41"/>
-    </row>
-    <row r="7" spans="1:9" ht="14.25" customHeight="1">
+      <c r="N6" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="41" t="s">
         <v>19</v>
       </c>
@@ -2381,8 +2720,12 @@
         <v>-125.3801</v>
       </c>
       <c r="I7" s="41"/>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1">
+      <c r="N7" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="46"/>
       <c r="B8" s="33" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A8),"""",filter(Moorings!A:A,Moorings!B:B=left(A8,14),Moorings!D:D=D8))"),"")</f>
@@ -2404,8 +2747,12 @@
       <c r="G8" s="37"/>
       <c r="H8" s="47"/>
       <c r="I8" s="37"/>
-    </row>
-    <row r="9" spans="1:9" ht="14.25" customHeight="1">
+      <c r="N8" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="48" t="s">
         <v>46</v>
       </c>
@@ -2437,8 +2784,12 @@
       <c r="I9" s="52" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="14.25" customHeight="1">
+      <c r="N9" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
         <v>46</v>
       </c>
@@ -2469,7 +2820,7 @@
       </c>
       <c r="I10" s="37"/>
     </row>
-    <row r="11" spans="1:9" ht="14.25" customHeight="1">
+    <row r="11" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="48" t="s">
         <v>46</v>
       </c>
@@ -2500,7 +2851,7 @@
       </c>
       <c r="I11" s="37"/>
     </row>
-    <row r="12" spans="1:9" ht="14.25" customHeight="1">
+    <row r="12" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="48" t="s">
         <v>46</v>
       </c>
@@ -2531,7 +2882,7 @@
       </c>
       <c r="I12" s="37"/>
     </row>
-    <row r="13" spans="1:9" ht="14.25" customHeight="1">
+    <row r="13" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="48" t="s">
         <v>46</v>
       </c>
@@ -2562,7 +2913,7 @@
       </c>
       <c r="I13" s="37"/>
     </row>
-    <row r="14" spans="1:9" ht="14.25" customHeight="1">
+    <row r="14" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="48" t="s">
         <v>46</v>
       </c>
@@ -2593,7 +2944,7 @@
       </c>
       <c r="I14" s="37"/>
     </row>
-    <row r="15" spans="1:9" ht="14.25" customHeight="1">
+    <row r="15" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="48" t="s">
         <v>46</v>
       </c>
@@ -2624,7 +2975,7 @@
       </c>
       <c r="I15" s="37"/>
     </row>
-    <row r="16" spans="1:9" ht="14.25" customHeight="1">
+    <row r="16" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="48" t="s">
         <v>46</v>
       </c>
@@ -2655,32 +3006,20 @@
       </c>
       <c r="I16" s="37"/>
     </row>
-    <row r="17" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A17" s="53"/>
-      <c r="B17" s="33" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A17),"""",filter(Moorings!A:A,Moorings!B:B=left(A17,14),Moorings!D:D=D17))"),"")</f>
-        <v/>
-      </c>
-      <c r="C17" s="34" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A17),"""",filter(Moorings!C:C,Moorings!B:B=left(A17,14),Moorings!D:D=D17))"),"")</f>
-        <v/>
-      </c>
-      <c r="D17" s="40"/>
-      <c r="E17" s="34" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A17),"""",filter(Moorings!A:A,Moorings!B:B=A17,Moorings!D:D=D17))"),"")</f>
-        <v/>
-      </c>
-      <c r="F17" s="34" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A17),"""",filter(Moorings!C:C,Moorings!B:B=A17,Moorings!D:D=D17))"),"")</f>
-        <v/>
-      </c>
-      <c r="G17" s="37"/>
-      <c r="H17" s="54"/>
+    <row r="17" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="50"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="51"/>
       <c r="I17" s="37"/>
     </row>
-    <row r="18" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A18" s="50" t="s">
-        <v>23</v>
+    <row r="18" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>112</v>
       </c>
       <c r="B18" s="38" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A18),"""",filter(Moorings!A:A,Moorings!B:B=left(A18,14),Moorings!D:D=D18))"),"ATAPL-71403-00002")</f>
@@ -2709,9 +3048,9 @@
       </c>
       <c r="I18" s="41"/>
     </row>
-    <row r="19" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A19" s="50" t="s">
-        <v>23</v>
+    <row r="19" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>112</v>
       </c>
       <c r="B19" s="38" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A19),"""",filter(Moorings!A:A,Moorings!B:B=left(A19,14),Moorings!D:D=D19))"),"ATAPL-71403-00002")</f>
@@ -2740,9 +3079,9 @@
       </c>
       <c r="I19" s="37"/>
     </row>
-    <row r="20" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A20" s="50" t="s">
-        <v>23</v>
+    <row r="20" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>112</v>
       </c>
       <c r="B20" s="38" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A20),"""",filter(Moorings!A:A,Moorings!B:B=left(A20,14),Moorings!D:D=D20))"),"ATAPL-71403-00002")</f>
@@ -2771,9 +3110,9 @@
       </c>
       <c r="I20" s="37"/>
     </row>
-    <row r="21" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A21" s="50" t="s">
-        <v>23</v>
+    <row r="21" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>112</v>
       </c>
       <c r="B21" s="38" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A21),"""",filter(Moorings!A:A,Moorings!B:B=left(A21,14),Moorings!D:D=D21))"),"ATAPL-71403-00002")</f>
@@ -2802,9 +3141,9 @@
       </c>
       <c r="I21" s="37"/>
     </row>
-    <row r="22" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A22" s="50" t="s">
-        <v>23</v>
+    <row r="22" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>112</v>
       </c>
       <c r="B22" s="38" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A22),"""",filter(Moorings!A:A,Moorings!B:B=left(A22,14),Moorings!D:D=D22))"),"ATAPL-71403-00002")</f>
@@ -2833,9 +3172,9 @@
       </c>
       <c r="I22" s="37"/>
     </row>
-    <row r="23" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A23" s="50" t="s">
-        <v>23</v>
+    <row r="23" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>112</v>
       </c>
       <c r="B23" s="38" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A23),"""",filter(Moorings!A:A,Moorings!B:B=left(A23,14),Moorings!D:D=D23))"),"ATAPL-71403-00002")</f>
@@ -2864,9 +3203,9 @@
       </c>
       <c r="I23" s="37"/>
     </row>
-    <row r="24" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A24" s="50" t="s">
-        <v>23</v>
+    <row r="24" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>112</v>
       </c>
       <c r="B24" s="38" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A24),"""",filter(Moorings!A:A,Moorings!B:B=left(A24,14),Moorings!D:D=D24))"),"ATAPL-71403-00002")</f>
@@ -2895,9 +3234,9 @@
       </c>
       <c r="I24" s="37"/>
     </row>
-    <row r="25" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A25" s="50" t="s">
-        <v>23</v>
+    <row r="25" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>112</v>
       </c>
       <c r="B25" s="38" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A25),"""",filter(Moorings!A:A,Moorings!B:B=left(A25,14),Moorings!D:D=D25))"),"ATAPL-71403-00002")</f>
@@ -2926,7 +3265,7 @@
       </c>
       <c r="I25" s="37"/>
     </row>
-    <row r="26" spans="1:9" ht="14.25" customHeight="1">
+    <row r="26" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="37"/>
       <c r="B26" s="33" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A26),"""",filter(Moorings!A:A,Moorings!B:B=left(A26,14),Moorings!D:D=D26))"),"")</f>
@@ -2949,9 +3288,9 @@
       <c r="H26" s="60"/>
       <c r="I26" s="37"/>
     </row>
-    <row r="27" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A27" s="50" t="s">
-        <v>48</v>
+    <row r="27" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>112</v>
       </c>
       <c r="B27" s="38" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A27),"""",filter(Moorings!A:A,Moorings!B:B=left(A27,14),Moorings!D:D=D27))"),"ATAPL-71403-00002")</f>
@@ -2980,9 +3319,9 @@
       </c>
       <c r="I27" s="37"/>
     </row>
-    <row r="28" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A28" s="50" t="s">
-        <v>48</v>
+    <row r="28" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>112</v>
       </c>
       <c r="B28" s="38" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A28),"""",filter(Moorings!A:A,Moorings!B:B=left(A28,14),Moorings!D:D=D28))"),"ATAPL-71403-00002")</f>
@@ -3011,9 +3350,9 @@
       </c>
       <c r="I28" s="37"/>
     </row>
-    <row r="29" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A29" s="50" t="s">
-        <v>48</v>
+    <row r="29" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>112</v>
       </c>
       <c r="B29" s="38" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A29),"""",filter(Moorings!A:A,Moorings!B:B=left(A29,14),Moorings!D:D=D29))"),"ATAPL-71403-00002")</f>
@@ -3042,9 +3381,9 @@
       </c>
       <c r="I29" s="37"/>
     </row>
-    <row r="30" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A30" s="50" t="s">
-        <v>48</v>
+    <row r="30" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>112</v>
       </c>
       <c r="B30" s="38" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A30),"""",filter(Moorings!A:A,Moorings!B:B=left(A30,14),Moorings!D:D=D30))"),"ATAPL-71403-00002")</f>
@@ -3073,9 +3412,9 @@
       </c>
       <c r="I30" s="37"/>
     </row>
-    <row r="31" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A31" s="50" t="s">
-        <v>48</v>
+    <row r="31" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>112</v>
       </c>
       <c r="B31" s="38" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A31),"""",filter(Moorings!A:A,Moorings!B:B=left(A31,14),Moorings!D:D=D31))"),"ATAPL-71403-00002")</f>
@@ -3104,9 +3443,9 @@
       </c>
       <c r="I31" s="37"/>
     </row>
-    <row r="32" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A32" s="50" t="s">
-        <v>48</v>
+    <row r="32" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>112</v>
       </c>
       <c r="B32" s="38" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A32),"""",filter(Moorings!A:A,Moorings!B:B=left(A32,14),Moorings!D:D=D32))"),"ATAPL-71403-00002")</f>
@@ -3135,9 +3474,9 @@
       </c>
       <c r="I32" s="37"/>
     </row>
-    <row r="33" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A33" s="50" t="s">
-        <v>48</v>
+    <row r="33" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>112</v>
       </c>
       <c r="B33" s="38" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A33),"""",filter(Moorings!A:A,Moorings!B:B=left(A33,14),Moorings!D:D=D33))"),"ATAPL-71403-00002")</f>
@@ -3166,9 +3505,9 @@
       </c>
       <c r="I33" s="37"/>
     </row>
-    <row r="34" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A34" s="50" t="s">
-        <v>48</v>
+    <row r="34" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>112</v>
       </c>
       <c r="B34" s="38" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A34),"""",filter(Moorings!A:A,Moorings!B:B=left(A34,14),Moorings!D:D=D34))"),"ATAPL-71403-00002")</f>
@@ -3197,7 +3536,7 @@
       </c>
       <c r="I34" s="37"/>
     </row>
-    <row r="35" spans="1:9" ht="15.75" customHeight="1">
+    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="53"/>
       <c r="B35" s="33" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A35),"""",filter(Moorings!A:A,Moorings!B:B=left(A35,14),Moorings!D:D=D35))"),"")</f>
@@ -3220,9 +3559,9 @@
       <c r="H35" s="47"/>
       <c r="I35" s="37"/>
     </row>
-    <row r="36" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A36" s="50" t="s">
-        <v>26</v>
+    <row r="36" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="66" t="s">
+        <v>50</v>
       </c>
       <c r="B36" s="38" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A36),"""",filter(Moorings!A:A,Moorings!B:B=left(A36,14),Moorings!D:D=D36))"),"ATAPL-71403-00002")</f>
@@ -3251,9 +3590,9 @@
       </c>
       <c r="I36" s="41"/>
     </row>
-    <row r="37" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A37" s="50" t="s">
-        <v>26</v>
+    <row r="37" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="66" t="s">
+        <v>50</v>
       </c>
       <c r="B37" s="38" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A37),"""",filter(Moorings!A:A,Moorings!B:B=left(A37,14),Moorings!D:D=D37))"),"ATAPL-71403-00002")</f>
@@ -3282,7 +3621,7 @@
       </c>
       <c r="I37" s="37"/>
     </row>
-    <row r="38" spans="1:9" ht="14.25" customHeight="1">
+    <row r="38" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="66"/>
       <c r="B38" s="33" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A38),"""",filter(Moorings!A:A,Moorings!B:B=left(A38,14),Moorings!D:D=D38))"),"")</f>
@@ -3305,7 +3644,7 @@
       <c r="H38" s="67"/>
       <c r="I38" s="37"/>
     </row>
-    <row r="39" spans="1:9" ht="14.25" customHeight="1">
+    <row r="39" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="66" t="s">
         <v>50</v>
       </c>
@@ -3336,7 +3675,7 @@
       </c>
       <c r="I39" s="37"/>
     </row>
-    <row r="40" spans="1:9" ht="14.25" customHeight="1">
+    <row r="40" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="66" t="s">
         <v>50</v>
       </c>
@@ -3367,7 +3706,7 @@
       </c>
       <c r="I40" s="37"/>
     </row>
-    <row r="41" spans="1:9" ht="15.75" customHeight="1">
+    <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="69"/>
       <c r="B41" s="33" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A41),"""",filter(Moorings!A:A,Moorings!B:B=left(A41,14),Moorings!D:D=D41))"),"")</f>
@@ -3390,7 +3729,7 @@
       <c r="H41" s="47"/>
       <c r="I41" s="37"/>
     </row>
-    <row r="42" spans="1:9" ht="14.25" customHeight="1">
+    <row r="42" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="41" t="s">
         <v>29</v>
       </c>
@@ -3421,7 +3760,7 @@
       </c>
       <c r="I42" s="41"/>
     </row>
-    <row r="43" spans="1:9" ht="14.25" customHeight="1">
+    <row r="43" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="41" t="s">
         <v>29</v>
       </c>
@@ -3452,7 +3791,7 @@
       </c>
       <c r="I43" s="41"/>
     </row>
-    <row r="44" spans="1:9" ht="14.25" customHeight="1">
+    <row r="44" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="41" t="s">
         <v>29</v>
       </c>
@@ -3483,7 +3822,7 @@
       </c>
       <c r="I44" s="41"/>
     </row>
-    <row r="45" spans="1:9" ht="14.25" customHeight="1">
+    <row r="45" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="41" t="s">
         <v>29</v>
       </c>
@@ -3514,7 +3853,7 @@
       </c>
       <c r="I45" s="41"/>
     </row>
-    <row r="46" spans="1:9" ht="14.25" customHeight="1">
+    <row r="46" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="41" t="s">
         <v>29</v>
       </c>
@@ -3545,7 +3884,7 @@
       </c>
       <c r="I46" s="41"/>
     </row>
-    <row r="47" spans="1:9" ht="14.25" customHeight="1">
+    <row r="47" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="37"/>
       <c r="B47" s="33" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A47),"""",filter(Moorings!A:A,Moorings!B:B=left(A47,14),Moorings!D:D=D47))"),"")</f>
@@ -3568,7 +3907,7 @@
       <c r="H47" s="47"/>
       <c r="I47" s="37"/>
     </row>
-    <row r="48" spans="1:9" ht="14.25" customHeight="1">
+    <row r="48" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="37" t="s">
         <v>29</v>
       </c>
@@ -3599,7 +3938,7 @@
       </c>
       <c r="I48" s="37"/>
     </row>
-    <row r="49" spans="1:9" ht="14.25" customHeight="1">
+    <row r="49" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="37" t="s">
         <v>29</v>
       </c>
@@ -3630,7 +3969,7 @@
       </c>
       <c r="I49" s="37"/>
     </row>
-    <row r="50" spans="1:9" ht="14.25" customHeight="1">
+    <row r="50" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="37" t="s">
         <v>29</v>
       </c>
@@ -3661,7 +4000,7 @@
       </c>
       <c r="I50" s="37"/>
     </row>
-    <row r="51" spans="1:9" ht="14.25" customHeight="1">
+    <row r="51" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="37" t="s">
         <v>29</v>
       </c>
@@ -3692,7 +4031,7 @@
       </c>
       <c r="I51" s="37"/>
     </row>
-    <row r="52" spans="1:9" ht="14.25" customHeight="1">
+    <row r="52" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="37" t="s">
         <v>29</v>
       </c>
@@ -3723,7 +4062,7 @@
       </c>
       <c r="I52" s="37"/>
     </row>
-    <row r="53" spans="1:9" ht="15.75" customHeight="1">
+    <row r="53" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="53"/>
       <c r="B53" s="33" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A53),"""",filter(Moorings!A:A,Moorings!B:B=left(A53,14),Moorings!D:D=D53))"),"")</f>
@@ -3746,7 +4085,7 @@
       <c r="H53" s="47"/>
       <c r="I53" s="37"/>
     </row>
-    <row r="54" spans="1:9" ht="14.25" customHeight="1">
+    <row r="54" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="75" t="s">
         <v>31</v>
       </c>
@@ -3777,7 +4116,7 @@
       </c>
       <c r="I54" s="37"/>
     </row>
-    <row r="55" spans="1:9" ht="14.25" customHeight="1">
+    <row r="55" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="75" t="s">
         <v>31</v>
       </c>
@@ -3808,7 +4147,7 @@
       </c>
       <c r="I55" s="37"/>
     </row>
-    <row r="56" spans="1:9" ht="15.75" customHeight="1">
+    <row r="56" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="53"/>
       <c r="B56" s="33" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A56),"""",filter(Moorings!A:A,Moorings!B:B=left(A56,14),Moorings!D:D=D56))"),"")</f>
@@ -3831,7 +4170,7 @@
       <c r="H56" s="47"/>
       <c r="I56" s="37"/>
     </row>
-    <row r="57" spans="1:9" ht="15.75" customHeight="1">
+    <row r="57" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="76" t="s">
         <v>31</v>
       </c>
@@ -3862,7 +4201,7 @@
       </c>
       <c r="I57" s="41"/>
     </row>
-    <row r="58" spans="1:9" ht="15.75" customHeight="1">
+    <row r="58" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="76" t="s">
         <v>31</v>
       </c>
@@ -3893,7 +4232,7 @@
       </c>
       <c r="I58" s="41"/>
     </row>
-    <row r="59" spans="1:9" ht="15.75" customHeight="1">
+    <row r="59" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="69"/>
       <c r="B59" s="33" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A59),"""",filter(Moorings!A:A,Moorings!B:B=left(A59,14),Moorings!D:D=D59))"),"")</f>
@@ -3918,28 +4257,58 @@
         <v>94</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A60" s="69"/>
-      <c r="B60" s="33" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A60),"""",filter(Moorings!A:A,Moorings!B:B=left(A60,14),Moorings!D:D=D60))"),"")</f>
-        <v/>
-      </c>
-      <c r="C60" s="34" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A60),"""",filter(Moorings!C:C,Moorings!B:B=left(A60,14),Moorings!D:D=D60))"),"")</f>
-        <v/>
-      </c>
-      <c r="D60" s="70"/>
-      <c r="E60" s="34" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A60),"""",filter(Moorings!A:A,Moorings!B:B=A60,Moorings!D:D=D60))"),"")</f>
-        <v/>
-      </c>
-      <c r="F60" s="34" t="str">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A60),"""",filter(Moorings!C:C,Moorings!B:B=A60,Moorings!D:D=D60))"),"")</f>
-        <v/>
+    <row r="60" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>111</v>
+      </c>
+      <c r="B60" s="38" t="str">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A58),"""",filter(Moorings!A:A,Moorings!B:B=left(A58,14),Moorings!D:D=D58))"),"ATAPL-71403-00002")</f>
+        <v>ATAPL-71403-00002</v>
+      </c>
+      <c r="C60" s="39" t="str">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A58),"""",filter(Moorings!C:C,Moorings!B:B=left(A58,14),Moorings!D:D=D58))"),"13152-03")</f>
+        <v>13152-03</v>
+      </c>
+      <c r="D60" s="70">
+        <v>1</v>
+      </c>
+      <c r="E60" s="98" t="s">
+        <v>115</v>
+      </c>
+      <c r="F60" t="s">
+        <v>113</v>
       </c>
       <c r="G60" s="68"/>
       <c r="H60" s="47"/>
       <c r="I60" s="37"/>
+    </row>
+    <row r="61" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>111</v>
+      </c>
+      <c r="B61" s="38" t="str">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A58),"""",filter(Moorings!A:A,Moorings!B:B=left(A58,14),Moorings!D:D=D58))"),"ATAPL-71403-00002")</f>
+        <v>ATAPL-71403-00002</v>
+      </c>
+      <c r="C61" s="39" t="str">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("if(isblank(A58),"""",filter(Moorings!C:C,Moorings!B:B=left(A58,14),Moorings!D:D=D58))"),"13152-03")</f>
+        <v>13152-03</v>
+      </c>
+      <c r="D61" s="97">
+        <v>2</v>
+      </c>
+      <c r="E61" s="98" t="s">
+        <v>116</v>
+      </c>
+      <c r="F61" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D62" s="97"/>
+    </row>
+    <row r="63" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D63" s="97"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3960,13 +4329,13 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" customWidth="1"/>
-    <col min="3" max="3" width="30.83203125" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>95</v>
       </c>
@@ -3989,7 +4358,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="78" t="str">
         <f>Moorings!A2</f>
         <v>ATAPL-71403-00002</v>
@@ -4016,7 +4385,7 @@
       </c>
       <c r="G2" s="79"/>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="78" t="str">
         <f>Moorings!A3</f>
         <v>ATAPL-58320-00002</v>
@@ -4043,7 +4412,7 @@
       </c>
       <c r="G3" s="79"/>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="78" t="str">
         <f>Moorings!A4</f>
         <v>ATAPL-70110-00001</v>
@@ -4054,7 +4423,7 @@
       </c>
       <c r="C4" s="78" t="str">
         <f>IF(D4="Sensor",Moorings!B4,"")</f>
-        <v>RS01SBPD-DP01A-04-FLNTUA102</v>
+        <v>RS01SBPD-DP01A-03-FLNTUA104</v>
       </c>
       <c r="D4" s="80" t="str">
         <f>IF(ISBLANK(Moorings!B4),"",IF(LEN(Moorings!B4)&gt;14,"Sensor","Mooring"))</f>
@@ -4070,7 +4439,7 @@
       </c>
       <c r="G4" s="79"/>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="78" t="str">
         <f>Moorings!A5</f>
         <v>ATAPL-70111-00001</v>
@@ -4081,7 +4450,7 @@
       </c>
       <c r="C5" s="78" t="str">
         <f>IF(D5="Sensor",Moorings!B5,"")</f>
-        <v>RS01SBPD-DP01A-03-FLCDRA102</v>
+        <v>RS01SBPD-DP01A-03-FLCDRA104</v>
       </c>
       <c r="D5" s="80" t="str">
         <f>IF(ISBLANK(Moorings!B5),"",IF(LEN(Moorings!B5)&gt;14,"Sensor","Mooring"))</f>
@@ -4097,7 +4466,7 @@
       </c>
       <c r="G5" s="79"/>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="78" t="str">
         <f>Moorings!A6</f>
         <v>ATAPL-58346-00001</v>
@@ -4124,7 +4493,7 @@
       </c>
       <c r="G6" s="79"/>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="78" t="str">
         <f>Moorings!A7</f>
         <v>ATAPL-67977-00001</v>
@@ -4151,7 +4520,7 @@
       </c>
       <c r="G7" s="79"/>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="78" t="str">
         <f>Moorings!A8</f>
         <v>ATAPL-71553-00002</v>
@@ -4178,353 +4547,353 @@
       </c>
       <c r="G8" s="79"/>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="78">
-        <f>Moorings!A9</f>
+        <f>Moorings!A10</f>
         <v>0</v>
       </c>
       <c r="B9" s="79" t="str">
-        <f>IF(D9="Mooring",Moorings!B9,"")</f>
+        <f>IF(D9="Mooring",Moorings!B10,"")</f>
         <v/>
       </c>
       <c r="C9" s="79" t="str">
-        <f>IF(D9="Sensor",Moorings!B9,"")</f>
+        <f>IF(D9="Sensor",Moorings!B10,"")</f>
         <v/>
       </c>
       <c r="D9" s="80" t="str">
-        <f>IF(ISBLANK(Moorings!B9),"",IF(LEN(Moorings!B9)&gt;14,"Sensor","Mooring"))</f>
+        <f>IF(ISBLANK(Moorings!B10),"",IF(LEN(Moorings!B10)&gt;14,"Sensor","Mooring"))</f>
         <v/>
       </c>
       <c r="E9" s="81">
-        <f>Moorings!C9</f>
+        <f>Moorings!C10</f>
         <v>0</v>
       </c>
       <c r="F9" s="82" t="str">
-        <f>IF(D9="Mooring",Moorings!E9,"")</f>
+        <f>IF(D9="Mooring",Moorings!E10,"")</f>
         <v/>
       </c>
       <c r="G9" s="79"/>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="78" t="str">
-        <f>Moorings!A10</f>
+        <f>Moorings!A11</f>
         <v>ATAPL-71403-00002</v>
       </c>
       <c r="B10" s="78" t="str">
-        <f>IF(D10="Mooring",Moorings!B10,"")</f>
+        <f>IF(D10="Mooring",Moorings!B11,"")</f>
         <v>RS01SBPD-DP01A</v>
       </c>
       <c r="C10" s="79" t="str">
-        <f>IF(D10="Sensor",Moorings!B10,"")</f>
+        <f>IF(D10="Sensor",Moorings!B11,"")</f>
         <v/>
       </c>
       <c r="D10" s="80" t="str">
-        <f>IF(ISBLANK(Moorings!B10),"",IF(LEN(Moorings!B10)&gt;14,"Sensor","Mooring"))</f>
+        <f>IF(ISBLANK(Moorings!B11),"",IF(LEN(Moorings!B11)&gt;14,"Sensor","Mooring"))</f>
         <v>Mooring</v>
       </c>
       <c r="E10" s="81" t="str">
-        <f>Moorings!C10</f>
+        <f>Moorings!C11</f>
         <v>13152-03</v>
       </c>
       <c r="F10" s="82">
-        <f>IF(D10="Mooring",Moorings!E10,"")</f>
+        <f>IF(D10="Mooring",Moorings!E11,"")</f>
         <v>42207</v>
       </c>
       <c r="G10" s="79"/>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="78" t="str">
-        <f>Moorings!A11</f>
+        <f>Moorings!A12</f>
         <v>ATAPL-58320-00010</v>
       </c>
       <c r="B11" s="79" t="str">
-        <f>IF(D11="Mooring",Moorings!B11,"")</f>
+        <f>IF(D11="Mooring",Moorings!B12,"")</f>
         <v/>
       </c>
       <c r="C11" s="78" t="str">
-        <f>IF(D11="Sensor",Moorings!B11,"")</f>
+        <f>IF(D11="Sensor",Moorings!B12,"")</f>
         <v>RS01SBPD-DP01A-06-DOSTAD104</v>
       </c>
       <c r="D11" s="80" t="str">
-        <f>IF(ISBLANK(Moorings!B11),"",IF(LEN(Moorings!B11)&gt;14,"Sensor","Mooring"))</f>
-        <v>Sensor</v>
-      </c>
-      <c r="E11" s="81">
-        <f>Moorings!C11</f>
-        <v>459</v>
-      </c>
-      <c r="F11" s="82" t="str">
-        <f>IF(D11="Mooring",Moorings!E11,"")</f>
-        <v/>
-      </c>
-      <c r="G11" s="79"/>
-    </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1">
-      <c r="A12" s="78" t="str">
-        <f>Moorings!A12</f>
-        <v>ATAPL-69943-00004</v>
-      </c>
-      <c r="B12" s="79" t="str">
-        <f>IF(D12="Mooring",Moorings!B12,"")</f>
-        <v/>
-      </c>
-      <c r="C12" s="78" t="str">
-        <f>IF(D12="Sensor",Moorings!B12,"")</f>
-        <v>RS01SBPD-DP01A-05-OPTAAC102</v>
-      </c>
-      <c r="D12" s="80" t="str">
         <f>IF(ISBLANK(Moorings!B12),"",IF(LEN(Moorings!B12)&gt;14,"Sensor","Mooring"))</f>
         <v>Sensor</v>
       </c>
-      <c r="E12" s="81">
+      <c r="E11" s="81">
         <f>Moorings!C12</f>
-        <v>158</v>
-      </c>
-      <c r="F12" s="82" t="str">
-        <f>IF(D12="Mooring",Moorings!E12,"")</f>
+        <v>459</v>
+      </c>
+      <c r="F11" s="82" t="str">
+        <f>IF(D11="Mooring",Moorings!E12,"")</f>
         <v/>
       </c>
-      <c r="G12" s="79"/>
-    </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1">
-      <c r="A13" s="78" t="str">
+      <c r="G11" s="79"/>
+    </row>
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="78" t="str">
         <f>Moorings!A13</f>
-        <v>ATAPL-70110-00004</v>
-      </c>
-      <c r="B13" s="79" t="str">
-        <f>IF(D13="Mooring",Moorings!B13,"")</f>
+        <v>ATAPL-69943-00004</v>
+      </c>
+      <c r="B12" s="79" t="str">
+        <f>IF(D12="Mooring",Moorings!B13,"")</f>
         <v/>
       </c>
-      <c r="C13" s="78" t="str">
-        <f>IF(D13="Sensor",Moorings!B13,"")</f>
-        <v>RS01SBPD-DP01A-04-FLNTUA104</v>
-      </c>
-      <c r="D13" s="80" t="str">
+      <c r="C12" s="78" t="str">
+        <f>IF(D12="Sensor",Moorings!B13,"")</f>
+        <v>RS01SBPD-DP01A-05-OPTAAC102</v>
+      </c>
+      <c r="D12" s="80" t="str">
         <f>IF(ISBLANK(Moorings!B13),"",IF(LEN(Moorings!B13)&gt;14,"Sensor","Mooring"))</f>
         <v>Sensor</v>
       </c>
-      <c r="E13" s="81">
+      <c r="E12" s="81">
         <f>Moorings!C13</f>
-        <v>3637</v>
-      </c>
-      <c r="F13" s="82" t="str">
-        <f>IF(D13="Mooring",Moorings!E13,"")</f>
+        <v>158</v>
+      </c>
+      <c r="F12" s="82" t="str">
+        <f>IF(D12="Mooring",Moorings!E13,"")</f>
         <v/>
       </c>
-      <c r="G13" s="79"/>
-    </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1">
-      <c r="A14" s="78" t="str">
+      <c r="G12" s="79"/>
+    </row>
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="78" t="str">
         <f>Moorings!A14</f>
-        <v>ATAPL-70111-00004</v>
-      </c>
-      <c r="B14" s="79" t="str">
-        <f>IF(D14="Mooring",Moorings!B14,"")</f>
+        <v>ATAPL-70110-00004</v>
+      </c>
+      <c r="B13" s="79" t="str">
+        <f>IF(D13="Mooring",Moorings!B14,"")</f>
         <v/>
       </c>
-      <c r="C14" s="78" t="str">
-        <f>IF(D14="Sensor",Moorings!B14,"")</f>
-        <v>RS01SBPD-DP01A-03-FLCDRA104</v>
-      </c>
-      <c r="D14" s="80" t="str">
+      <c r="C13" s="78" t="str">
+        <f>IF(D13="Sensor",Moorings!B14,"")</f>
+        <v>RS01SBPD-DP01A-03-FLNTUA104</v>
+      </c>
+      <c r="D13" s="80" t="str">
         <f>IF(ISBLANK(Moorings!B14),"",IF(LEN(Moorings!B14)&gt;14,"Sensor","Mooring"))</f>
         <v>Sensor</v>
       </c>
-      <c r="E14" s="81">
+      <c r="E13" s="81">
         <f>Moorings!C14</f>
-        <v>3715</v>
-      </c>
-      <c r="F14" s="82" t="str">
-        <f>IF(D14="Mooring",Moorings!E14,"")</f>
+        <v>3637</v>
+      </c>
+      <c r="F13" s="82" t="str">
+        <f>IF(D13="Mooring",Moorings!E14,"")</f>
         <v/>
       </c>
-      <c r="G14" s="79"/>
-    </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1">
-      <c r="A15" s="78" t="str">
+      <c r="G13" s="79"/>
+    </row>
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="78" t="str">
         <f>Moorings!A15</f>
-        <v>ATAPL-58346-00006</v>
-      </c>
-      <c r="B15" s="79" t="str">
-        <f>IF(D15="Mooring",Moorings!B15,"")</f>
+        <v>ATAPL-70111-00004</v>
+      </c>
+      <c r="B14" s="79" t="str">
+        <f>IF(D14="Mooring",Moorings!B15,"")</f>
         <v/>
       </c>
-      <c r="C15" s="78" t="str">
-        <f>IF(D15="Sensor",Moorings!B15,"")</f>
-        <v>RS01SBPD-DP01A-02-VEL3DA103</v>
-      </c>
-      <c r="D15" s="80" t="str">
+      <c r="C14" s="78" t="str">
+        <f>IF(D14="Sensor",Moorings!B15,"")</f>
+        <v>RS01SBPD-DP01A-03-FLCDRA104</v>
+      </c>
+      <c r="D14" s="80" t="str">
         <f>IF(ISBLANK(Moorings!B15),"",IF(LEN(Moorings!B15)&gt;14,"Sensor","Mooring"))</f>
         <v>Sensor</v>
       </c>
-      <c r="E15" s="81">
+      <c r="E14" s="81">
         <f>Moorings!C15</f>
-        <v>1215</v>
-      </c>
-      <c r="F15" s="82" t="str">
-        <f>IF(D15="Mooring",Moorings!E15,"")</f>
+        <v>3715</v>
+      </c>
+      <c r="F14" s="82" t="str">
+        <f>IF(D14="Mooring",Moorings!E15,"")</f>
         <v/>
       </c>
-      <c r="G15" s="79"/>
-    </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1">
-      <c r="A16" s="78" t="str">
+      <c r="G14" s="79"/>
+    </row>
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="78" t="str">
         <f>Moorings!A16</f>
-        <v>ATAPL-67977-00004</v>
-      </c>
-      <c r="B16" s="79" t="str">
-        <f>IF(D16="Mooring",Moorings!B16,"")</f>
+        <v>ATAPL-58346-00006</v>
+      </c>
+      <c r="B15" s="79" t="str">
+        <f>IF(D15="Mooring",Moorings!B16,"")</f>
         <v/>
       </c>
-      <c r="C16" s="78" t="str">
-        <f>IF(D16="Sensor",Moorings!B16,"")</f>
-        <v>RS01SBPD-DP01A-01-CTDPFL104</v>
-      </c>
-      <c r="D16" s="80" t="str">
+      <c r="C15" s="78" t="str">
+        <f>IF(D15="Sensor",Moorings!B16,"")</f>
+        <v>RS01SBPD-DP01A-02-VEL3DA103</v>
+      </c>
+      <c r="D15" s="80" t="str">
         <f>IF(ISBLANK(Moorings!B16),"",IF(LEN(Moorings!B16)&gt;14,"Sensor","Mooring"))</f>
         <v>Sensor</v>
       </c>
+      <c r="E15" s="81">
+        <f>Moorings!C16</f>
+        <v>1215</v>
+      </c>
+      <c r="F15" s="82" t="str">
+        <f>IF(D15="Mooring",Moorings!E16,"")</f>
+        <v/>
+      </c>
+      <c r="G15" s="79"/>
+    </row>
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="78" t="str">
+        <f>Moorings!A17</f>
+        <v>ATAPL-67977-00004</v>
+      </c>
+      <c r="B16" s="79" t="str">
+        <f>IF(D16="Mooring",Moorings!B17,"")</f>
+        <v/>
+      </c>
+      <c r="C16" s="78" t="str">
+        <f>IF(D16="Sensor",Moorings!B17,"")</f>
+        <v>RS01SBPD-DP01A-01-CTDPFL104</v>
+      </c>
+      <c r="D16" s="80" t="str">
+        <f>IF(ISBLANK(Moorings!B17),"",IF(LEN(Moorings!B17)&gt;14,"Sensor","Mooring"))</f>
+        <v>Sensor</v>
+      </c>
       <c r="E16" s="81" t="str">
-        <f>Moorings!C16</f>
+        <f>Moorings!C17</f>
         <v>52-0144</v>
       </c>
       <c r="F16" s="82" t="str">
-        <f>IF(D16="Mooring",Moorings!E16,"")</f>
+        <f>IF(D16="Mooring",Moorings!E17,"")</f>
         <v/>
       </c>
       <c r="G16" s="79"/>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="78" t="str">
-        <f>Moorings!A17</f>
+        <f>Moorings!A18</f>
         <v>ATAPL-71553-00002</v>
       </c>
       <c r="B17" s="78" t="str">
-        <f>IF(D17="Mooring",Moorings!B17,"")</f>
+        <f>IF(D17="Mooring",Moorings!B18,"")</f>
         <v>RS01SBPD-PD01A</v>
       </c>
       <c r="C17" s="79" t="str">
-        <f>IF(D17="Sensor",Moorings!B17,"")</f>
+        <f>IF(D17="Sensor",Moorings!B18,"")</f>
         <v/>
       </c>
       <c r="D17" s="80" t="str">
-        <f>IF(ISBLANK(Moorings!B17),"",IF(LEN(Moorings!B17)&gt;14,"Sensor","Mooring"))</f>
+        <f>IF(ISBLANK(Moorings!B18),"",IF(LEN(Moorings!B18)&gt;14,"Sensor","Mooring"))</f>
         <v>Mooring</v>
       </c>
       <c r="E17" s="81" t="str">
-        <f>Moorings!C17</f>
+        <f>Moorings!C18</f>
         <v>SN0003</v>
       </c>
       <c r="F17" s="82">
-        <f>IF(D17="Mooring",Moorings!E17,"")</f>
+        <f>IF(D17="Mooring",Moorings!E18,"")</f>
         <v>42207</v>
       </c>
       <c r="G17" s="79"/>
     </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1">
-      <c r="A18" s="78">
-        <f>Moorings!A18</f>
-        <v>0</v>
-      </c>
-      <c r="B18" s="79" t="str">
-        <f>IF(D18="Mooring",Moorings!B18,"")</f>
-        <v/>
-      </c>
-      <c r="C18" s="79" t="str">
-        <f>IF(D18="Sensor",Moorings!B18,"")</f>
-        <v/>
-      </c>
-      <c r="D18" s="80" t="str">
-        <f>IF(ISBLANK(Moorings!B18),"",IF(LEN(Moorings!B18)&gt;14,"Sensor","Mooring"))</f>
-        <v/>
-      </c>
-      <c r="E18" s="81">
-        <f>Moorings!C18</f>
-        <v>0</v>
-      </c>
-      <c r="F18" s="82" t="str">
-        <f>IF(D18="Mooring",Moorings!E18,"")</f>
-        <v/>
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="78" t="e">
+        <f>Moorings!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B18" s="79" t="e">
+        <f>IF(D18="Mooring",Moorings!#REF!,"")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C18" s="79" t="e">
+        <f>IF(D18="Sensor",Moorings!#REF!,"")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D18" s="80" t="e">
+        <f>IF(ISBLANK(Moorings!#REF!),"",IF(LEN(Moorings!#REF!)&gt;14,"Sensor","Mooring"))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E18" s="81" t="str">
+        <f>Moorings!C19</f>
+        <v>RS01SBPD-DP01A-ENG-00002</v>
+      </c>
+      <c r="F18" s="82" t="e">
+        <f>IF(D18="Mooring",Moorings!E19,"")</f>
+        <v>#REF!</v>
       </c>
       <c r="G18" s="79"/>
     </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1">
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="78">
-        <f>Moorings!A19</f>
-        <v>0</v>
-      </c>
-      <c r="B19" s="79" t="str">
-        <f>IF(D19="Mooring",Moorings!B19,"")</f>
-        <v/>
-      </c>
-      <c r="C19" s="79" t="str">
-        <f>IF(D19="Sensor",Moorings!B19,"")</f>
-        <v/>
-      </c>
-      <c r="D19" s="80" t="str">
-        <f>IF(ISBLANK(Moorings!B19),"",IF(LEN(Moorings!B19)&gt;14,"Sensor","Mooring"))</f>
-        <v/>
-      </c>
-      <c r="E19" s="81">
-        <f>Moorings!C19</f>
-        <v>0</v>
-      </c>
-      <c r="F19" s="82" t="str">
-        <f>IF(D19="Mooring",Moorings!E19,"")</f>
-        <v/>
-      </c>
-      <c r="G19" s="79"/>
-    </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1">
-      <c r="A20" s="78">
         <f>Moorings!A20</f>
         <v>0</v>
       </c>
-      <c r="B20" s="79" t="str">
-        <f>IF(D20="Mooring",Moorings!B20,"")</f>
+      <c r="B19" s="79" t="str">
+        <f>IF(D19="Mooring",Moorings!B20,"")</f>
         <v/>
       </c>
-      <c r="C20" s="79" t="str">
-        <f>IF(D20="Sensor",Moorings!B20,"")</f>
+      <c r="C19" s="79" t="str">
+        <f>IF(D19="Sensor",Moorings!B20,"")</f>
         <v/>
       </c>
-      <c r="D20" s="80" t="str">
+      <c r="D19" s="80" t="str">
         <f>IF(ISBLANK(Moorings!B20),"",IF(LEN(Moorings!B20)&gt;14,"Sensor","Mooring"))</f>
         <v/>
       </c>
-      <c r="E20" s="81">
+      <c r="E19" s="81">
         <f>Moorings!C20</f>
         <v>0</v>
       </c>
-      <c r="F20" s="82" t="str">
-        <f>IF(D20="Mooring",Moorings!E20,"")</f>
+      <c r="F19" s="82" t="str">
+        <f>IF(D19="Mooring",Moorings!E20,"")</f>
         <v/>
       </c>
-      <c r="G20" s="79"/>
-    </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1">
-      <c r="A21" s="78">
+      <c r="G19" s="79"/>
+    </row>
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="78">
         <f>Moorings!A21</f>
         <v>0</v>
       </c>
-      <c r="B21" s="79" t="str">
-        <f>IF(D21="Mooring",Moorings!B21,"")</f>
+      <c r="B20" s="79" t="str">
+        <f>IF(D20="Mooring",Moorings!B21,"")</f>
         <v/>
       </c>
-      <c r="C21" s="79" t="str">
-        <f>IF(D21="Sensor",Moorings!B21,"")</f>
+      <c r="C20" s="79" t="str">
+        <f>IF(D20="Sensor",Moorings!B21,"")</f>
         <v/>
       </c>
-      <c r="D21" s="80" t="str">
+      <c r="D20" s="80" t="str">
         <f>IF(ISBLANK(Moorings!B21),"",IF(LEN(Moorings!B21)&gt;14,"Sensor","Mooring"))</f>
         <v/>
       </c>
-      <c r="E21" s="81">
+      <c r="E20" s="81">
         <f>Moorings!C21</f>
         <v>0</v>
       </c>
+      <c r="F20" s="82" t="str">
+        <f>IF(D20="Mooring",Moorings!E21,"")</f>
+        <v/>
+      </c>
+      <c r="G20" s="79"/>
+    </row>
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="78" t="str">
+        <f>Moorings!A9</f>
+        <v>OL000577</v>
+      </c>
+      <c r="B21" s="79" t="str">
+        <f>IF(D21="Mooring",Moorings!B22,"")</f>
+        <v/>
+      </c>
+      <c r="C21" s="79" t="str">
+        <f>IF(D21="Sensor",Moorings!B22,"")</f>
+        <v/>
+      </c>
+      <c r="D21" s="80" t="str">
+        <f>IF(ISBLANK(Moorings!B22),"",IF(LEN(Moorings!B22)&gt;14,"Sensor","Mooring"))</f>
+        <v/>
+      </c>
+      <c r="E21" s="81">
+        <f>Moorings!C22</f>
+        <v>0</v>
+      </c>
       <c r="F21" s="82" t="str">
-        <f>IF(D21="Mooring",Moorings!E21,"")</f>
+        <f>IF(D21="Mooring",Moorings!E22,"")</f>
         <v/>
       </c>
       <c r="G21" s="79"/>
@@ -4545,18 +4914,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.5" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
     <col min="3" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="5.6640625" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="19.5" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="83" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("sort(unique(Moorings!B:B))"),"Ref Des")</f>
         <v>Ref Des</v>
@@ -4584,7 +4953,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -4601,7 +4970,7 @@
       <c r="H2" s="89"/>
       <c r="I2" s="88"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -4622,7 +4991,7 @@
       <c r="H3" s="90"/>
       <c r="I3" s="87"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -4643,7 +5012,7 @@
       <c r="H4" s="90"/>
       <c r="I4" s="88"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -4664,7 +5033,7 @@
       <c r="H5" s="89"/>
       <c r="I5" s="88"/>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -4685,7 +5054,7 @@
       <c r="H6" s="90"/>
       <c r="I6" s="88"/>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -4706,7 +5075,7 @@
       <c r="H7" s="90"/>
       <c r="I7" s="88"/>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1">
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -4727,7 +5096,7 @@
       <c r="H8" s="89"/>
       <c r="I8" s="88"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1">
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -4748,7 +5117,7 @@
       <c r="H9" s="90"/>
       <c r="I9" s="88"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1">
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -4769,7 +5138,7 @@
       <c r="H10" s="90"/>
       <c r="I10" s="88"/>
     </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1">
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -4788,7 +5157,7 @@
       <c r="H11" s="89"/>
       <c r="I11" s="88"/>
     </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1">
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="90"/>
       <c r="C12" s="87"/>
       <c r="D12" s="87"/>
@@ -4798,7 +5167,7 @@
       <c r="H12" s="91"/>
       <c r="I12" s="87"/>
     </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1">
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="92"/>
       <c r="C13" s="87"/>
       <c r="D13" s="87"/>
@@ -4808,7 +5177,7 @@
       <c r="H13" s="90"/>
       <c r="I13" s="87"/>
     </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1">
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="93" t="s">
         <v>110</v>
       </c>
@@ -4821,7 +5190,7 @@
       <c r="H14" s="90"/>
       <c r="I14" s="87"/>
     </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1">
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="90"/>
       <c r="C15" s="87"/>
       <c r="D15" s="87"/>
@@ -4831,7 +5200,7 @@
       <c r="H15" s="90"/>
       <c r="I15" s="87"/>
     </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1">
+    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="90"/>
       <c r="C16" s="87"/>
       <c r="D16" s="87"/>
@@ -4841,7 +5210,7 @@
       <c r="H16" s="90"/>
       <c r="I16" s="87"/>
     </row>
-    <row r="17" spans="1:9" ht="15" customHeight="1">
+    <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="93"/>
       <c r="B17" s="90"/>
       <c r="C17" s="87"/>
@@ -4852,7 +5221,7 @@
       <c r="H17" s="90"/>
       <c r="I17" s="88"/>
     </row>
-    <row r="18" spans="1:9" ht="15" customHeight="1">
+    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="93"/>
       <c r="B18" s="90"/>
       <c r="C18" s="87"/>
@@ -4863,7 +5232,7 @@
       <c r="H18" s="90"/>
       <c r="I18" s="88"/>
     </row>
-    <row r="19" spans="1:9" ht="15" customHeight="1">
+    <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="93"/>
       <c r="B19" s="90"/>
       <c r="C19" s="87"/>
@@ -4874,7 +5243,7 @@
       <c r="H19" s="90"/>
       <c r="I19" s="88"/>
     </row>
-    <row r="20" spans="1:9" ht="15" customHeight="1">
+    <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="93"/>
       <c r="B20" s="90"/>
       <c r="C20" s="87"/>
@@ -4885,7 +5254,7 @@
       <c r="H20" s="90"/>
       <c r="I20" s="88"/>
     </row>
-    <row r="21" spans="1:9" ht="15" customHeight="1">
+    <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="93"/>
       <c r="B21" s="90"/>
       <c r="C21" s="87"/>
@@ -4896,7 +5265,7 @@
       <c r="H21" s="90"/>
       <c r="I21" s="88"/>
     </row>
-    <row r="22" spans="1:9" ht="15" customHeight="1">
+    <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="93"/>
       <c r="B22" s="90"/>
       <c r="C22" s="87"/>
@@ -4907,7 +5276,7 @@
       <c r="H22" s="90"/>
       <c r="I22" s="88"/>
     </row>
-    <row r="23" spans="1:9" ht="15" customHeight="1">
+    <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="93"/>
       <c r="B23" s="94" t="str">
         <f>CONCATENATE("'",COUNTIF(B2:B22,"yes"),"/",COUNTA(B2:B22))</f>
@@ -4927,7 +5296,7 @@
       <c r="H23" s="90"/>
       <c r="I23" s="88"/>
     </row>
-    <row r="24" spans="1:9" ht="15" customHeight="1">
+    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="93"/>
       <c r="B24" s="90"/>
       <c r="C24" s="87"/>
@@ -4938,7 +5307,7 @@
       <c r="H24" s="90"/>
       <c r="I24" s="88"/>
     </row>
-    <row r="25" spans="1:9" ht="15" customHeight="1">
+    <row r="25" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="93"/>
       <c r="B25" s="90"/>
       <c r="C25" s="87"/>
@@ -4949,7 +5318,7 @@
       <c r="H25" s="90"/>
       <c r="I25" s="88"/>
     </row>
-    <row r="26" spans="1:9" ht="15" customHeight="1">
+    <row r="26" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="93"/>
       <c r="B26" s="90"/>
       <c r="C26" s="87"/>
@@ -4976,9 +5345,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:36" ht="15" customHeight="1">
+    <row r="1" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="93">
         <v>7.1318999999999994E-2</v>
       </c>
@@ -5088,7 +5457,7 @@
         <v>-3.4812999999999997E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="15" customHeight="1">
+    <row r="2" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="93">
         <v>6.2142000000000003E-2</v>
       </c>
@@ -5198,7 +5567,7 @@
         <v>-2.8777E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="15" customHeight="1">
+    <row r="3" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="93">
         <v>5.0567000000000001E-2</v>
       </c>
@@ -5308,7 +5677,7 @@
         <v>-2.4282999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:36" ht="15" customHeight="1">
+    <row r="4" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="93">
         <v>4.2000000000000003E-2</v>
       </c>
@@ -5418,7 +5787,7 @@
         <v>-2.0288E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:36" ht="15" customHeight="1">
+    <row r="5" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="93">
         <v>3.3696999999999998E-2</v>
       </c>
@@ -5528,7 +5897,7 @@
         <v>-1.7048000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:36" ht="15" customHeight="1">
+    <row r="6" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="93">
         <v>2.4523E-2</v>
       </c>
@@ -5638,7 +6007,7 @@
         <v>-1.3679999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:36" ht="15" customHeight="1">
+    <row r="7" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="93">
         <v>1.8377999999999999E-2</v>
       </c>
@@ -5748,7 +6117,7 @@
         <v>-1.0621999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:36" ht="15" customHeight="1">
+    <row r="8" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="93">
         <v>1.3573E-2</v>
       </c>
@@ -5858,7 +6227,7 @@
         <v>-8.7279999999999996E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:36" ht="15" customHeight="1">
+    <row r="9" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="93">
         <v>1.0711E-2</v>
       </c>
@@ -5968,7 +6337,7 @@
         <v>-6.3049999999999998E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:36" ht="15" customHeight="1">
+    <row r="10" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="93">
         <v>7.339E-3</v>
       </c>
@@ -6078,7 +6447,7 @@
         <v>-3.9150000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:36" ht="15" customHeight="1">
+    <row r="11" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="93">
         <v>4.509E-3</v>
       </c>
@@ -6188,7 +6557,7 @@
         <v>-2.843E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:36" ht="15" customHeight="1">
+    <row r="12" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="93">
         <v>3.8560000000000001E-3</v>
       </c>
@@ -6298,7 +6667,7 @@
         <v>-1.7979999999999999E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:36" ht="15" customHeight="1">
+    <row r="13" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="93">
         <v>1.645E-3</v>
       </c>
@@ -6408,7 +6777,7 @@
         <v>-6.4999999999999997E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:36" ht="15" customHeight="1">
+    <row r="14" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="93">
         <v>1.5759999999999999E-3</v>
       </c>
@@ -6518,7 +6887,7 @@
         <v>-7.7399999999999995E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:36" ht="15" customHeight="1">
+    <row r="15" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="93">
         <v>-8.2999999999999998E-5</v>
       </c>
@@ -6628,7 +6997,7 @@
         <v>-2.7E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:36" ht="15" customHeight="1">
+    <row r="16" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="93">
         <v>2.2800000000000001E-4</v>
       </c>
@@ -6738,7 +7107,7 @@
         <v>-5.5999999999999995E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:36" ht="15" customHeight="1">
+    <row r="17" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="93">
         <v>7.6300000000000001E-4</v>
       </c>
@@ -6848,7 +7217,7 @@
         <v>-7.4700000000000005E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:36" ht="15" customHeight="1">
+    <row r="18" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="93">
         <v>2.9399999999999999E-4</v>
       </c>
@@ -6958,7 +7327,7 @@
         <v>-8.7200000000000005E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:36" ht="15" customHeight="1">
+    <row r="19" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="93">
         <v>7.9799999999999999E-4</v>
       </c>
@@ -7068,7 +7437,7 @@
         <v>-1.1429999999999999E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:36" ht="15" customHeight="1">
+    <row r="20" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="93">
         <v>5.1699999999999999E-4</v>
       </c>
@@ -7178,7 +7547,7 @@
         <v>-1.1310000000000001E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:36" ht="15" customHeight="1">
+    <row r="21" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="93">
         <v>2.52E-4</v>
       </c>
@@ -7288,7 +7657,7 @@
         <v>-1.3749999999999999E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:36" ht="15" customHeight="1">
+    <row r="22" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="93">
         <v>6.5399999999999996E-4</v>
       </c>
@@ -7398,7 +7767,7 @@
         <v>-1.472E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:36" ht="15" customHeight="1">
+    <row r="23" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="93">
         <v>8.8599999999999996E-4</v>
       </c>
@@ -7508,7 +7877,7 @@
         <v>-1.7420000000000001E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:36" ht="15" customHeight="1">
+    <row r="24" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="93">
         <v>7.2999999999999996E-4</v>
       </c>
@@ -7618,7 +7987,7 @@
         <v>-1.8910000000000001E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:36" ht="15" customHeight="1">
+    <row r="25" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="93">
         <v>6.87E-4</v>
       </c>
@@ -7728,7 +8097,7 @@
         <v>-2.1570000000000001E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:36" ht="15" customHeight="1">
+    <row r="26" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="93">
         <v>8.3299999999999997E-4</v>
       </c>
@@ -7838,7 +8207,7 @@
         <v>-2.251E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:36" ht="15" customHeight="1">
+    <row r="27" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="93">
         <v>4.73E-4</v>
       </c>
@@ -7948,7 +8317,7 @@
         <v>-2.3969999999999998E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:36" ht="15" customHeight="1">
+    <row r="28" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="93">
         <v>5.4199999999999995E-4</v>
       </c>
@@ -8058,7 +8427,7 @@
         <v>-2.6589999999999999E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:36" ht="15" customHeight="1">
+    <row r="29" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="93">
         <v>6.6399999999999999E-4</v>
       </c>
@@ -8168,7 +8537,7 @@
         <v>-2.689E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:36" ht="15" customHeight="1">
+    <row r="30" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="93">
         <v>1.091E-3</v>
       </c>
@@ -8278,7 +8647,7 @@
         <v>-3.026E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:36" ht="15" customHeight="1">
+    <row r="31" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="93">
         <v>1.469E-3</v>
       </c>
@@ -8388,7 +8757,7 @@
         <v>-3.1740000000000002E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:36" ht="15" customHeight="1">
+    <row r="32" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="93">
         <v>1.1299999999999999E-3</v>
       </c>
@@ -8498,7 +8867,7 @@
         <v>-3.3860000000000001E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:36" ht="15" customHeight="1">
+    <row r="33" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="93">
         <v>1.5479999999999999E-3</v>
       </c>
@@ -8608,7 +8977,7 @@
         <v>-3.4589999999999998E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:36" ht="15" customHeight="1">
+    <row r="34" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="93">
         <v>2.3419999999999999E-3</v>
       </c>
@@ -8718,7 +9087,7 @@
         <v>-3.6700000000000001E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:36" ht="15" customHeight="1">
+    <row r="35" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="93">
         <v>2.3029999999999999E-3</v>
       </c>
@@ -8828,7 +9197,7 @@
         <v>-3.8769999999999998E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:36" ht="15" customHeight="1">
+    <row r="36" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="93">
         <v>2.6649999999999998E-3</v>
       </c>
@@ -8938,7 +9307,7 @@
         <v>-3.954E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:36" ht="15" customHeight="1">
+    <row r="37" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="93">
         <v>3.0599999999999998E-3</v>
       </c>
@@ -9048,7 +9417,7 @@
         <v>-3.9919999999999999E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:36" ht="15" customHeight="1">
+    <row r="38" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="93">
         <v>3.5109999999999998E-3</v>
       </c>
@@ -9158,7 +9527,7 @@
         <v>-4.1180000000000001E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:36" ht="15" customHeight="1">
+    <row r="39" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="93">
         <v>4.1159999999999999E-3</v>
       </c>
@@ -9268,7 +9637,7 @@
         <v>-4.2770000000000004E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:36" ht="15" customHeight="1">
+    <row r="40" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="93">
         <v>5.1390000000000003E-3</v>
       </c>
@@ -9378,7 +9747,7 @@
         <v>-4.2700000000000004E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:36" ht="15" customHeight="1">
+    <row r="41" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="93">
         <v>5.3330000000000001E-3</v>
       </c>
@@ -9488,7 +9857,7 @@
         <v>-4.7540000000000004E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:36" ht="15" customHeight="1">
+    <row r="42" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="93">
         <v>5.7419999999999997E-3</v>
       </c>
@@ -9598,7 +9967,7 @@
         <v>-4.6860000000000001E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:36" ht="15" customHeight="1">
+    <row r="43" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="93">
         <v>6.5050000000000004E-3</v>
       </c>
@@ -9708,7 +10077,7 @@
         <v>-5.4450000000000002E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:36" ht="15" customHeight="1">
+    <row r="44" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="93">
         <v>6.927E-3</v>
       </c>
@@ -9818,7 +10187,7 @@
         <v>-5.6420000000000003E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:36" ht="15" customHeight="1">
+    <row r="45" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="93">
         <v>7.2909999999999997E-3</v>
       </c>
@@ -9928,7 +10297,7 @@
         <v>-5.8079999999999998E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:36" ht="15" customHeight="1">
+    <row r="46" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="93">
         <v>7.6140000000000001E-3</v>
       </c>
@@ -10038,7 +10407,7 @@
         <v>-6.0130000000000001E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:36" ht="15" customHeight="1">
+    <row r="47" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="93">
         <v>7.8279999999999999E-3</v>
       </c>
@@ -10148,7 +10517,7 @@
         <v>-5.9659999999999999E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:36" ht="15" customHeight="1">
+    <row r="48" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="93">
         <v>8.6289999999999995E-3</v>
       </c>
@@ -10258,7 +10627,7 @@
         <v>-6.2519999999999997E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:36" ht="15" customHeight="1">
+    <row r="49" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="93">
         <v>8.5330000000000007E-3</v>
       </c>
@@ -10368,7 +10737,7 @@
         <v>-6.202E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:36" ht="15" customHeight="1">
+    <row r="50" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="93">
         <v>8.9409999999999993E-3</v>
       </c>
@@ -10478,7 +10847,7 @@
         <v>-6.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:36" ht="15" customHeight="1">
+    <row r="51" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="93">
         <v>9.0519999999999993E-3</v>
       </c>
@@ -10588,7 +10957,7 @@
         <v>-6.136E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:36" ht="15" customHeight="1">
+    <row r="52" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="93">
         <v>9.3710000000000009E-3</v>
       </c>
@@ -10698,7 +11067,7 @@
         <v>-6.0219999999999996E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:36" ht="15" customHeight="1">
+    <row r="53" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="93">
         <v>9.4870000000000006E-3</v>
       </c>
@@ -10808,7 +11177,7 @@
         <v>-5.8529999999999997E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:36" ht="15" customHeight="1">
+    <row r="54" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="93">
         <v>9.5700000000000004E-3</v>
       </c>
@@ -10918,7 +11287,7 @@
         <v>-5.7390000000000002E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:36" ht="15" customHeight="1">
+    <row r="55" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="93">
         <v>9.8519999999999996E-3</v>
       </c>
@@ -11028,7 +11397,7 @@
         <v>-5.6750000000000004E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:36" ht="15" customHeight="1">
+    <row r="56" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="93">
         <v>1.0064E-2</v>
       </c>
@@ -11138,7 +11507,7 @@
         <v>-5.3689999999999996E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:36" ht="15" customHeight="1">
+    <row r="57" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="93">
         <v>1.0035000000000001E-2</v>
       </c>
@@ -11248,7 +11617,7 @@
         <v>-5.2100000000000002E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:36" ht="15" customHeight="1">
+    <row r="58" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="93">
         <v>1.0463E-2</v>
       </c>
@@ -11358,7 +11727,7 @@
         <v>-4.9459999999999999E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:36" ht="15" customHeight="1">
+    <row r="59" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="93">
         <v>1.0633999999999999E-2</v>
       </c>
@@ -11468,7 +11837,7 @@
         <v>-4.8199999999999996E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:36" ht="15" customHeight="1">
+    <row r="60" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="93">
         <v>1.0954999999999999E-2</v>
       </c>
@@ -11578,7 +11947,7 @@
         <v>-4.7070000000000002E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:36" ht="15" customHeight="1">
+    <row r="61" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="93">
         <v>1.1344999999999999E-2</v>
       </c>
@@ -11688,7 +12057,7 @@
         <v>-4.3949999999999996E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:36" ht="15" customHeight="1">
+    <row r="62" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="93">
         <v>1.0295E-2</v>
       </c>
@@ -11798,7 +12167,7 @@
         <v>-3.441E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:36" ht="15" customHeight="1">
+    <row r="63" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="93">
         <v>1.1551000000000001E-2</v>
       </c>
@@ -11908,7 +12277,7 @@
         <v>-3.9560000000000003E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:36" ht="15" customHeight="1">
+    <row r="64" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="93">
         <v>1.1719E-2</v>
       </c>
@@ -12018,7 +12387,7 @@
         <v>-4.1050000000000001E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:36" ht="15" customHeight="1">
+    <row r="65" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="93">
         <v>1.2154999999999999E-2</v>
       </c>
@@ -12128,7 +12497,7 @@
         <v>-4.1050000000000001E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:36" ht="15" customHeight="1">
+    <row r="66" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="93">
         <v>1.2670000000000001E-2</v>
       </c>
@@ -12238,7 +12607,7 @@
         <v>-4.2360000000000002E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:36" ht="15" customHeight="1">
+    <row r="67" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="93">
         <v>1.3243E-2</v>
       </c>
@@ -12348,7 +12717,7 @@
         <v>-4.5459999999999997E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:36" ht="15" customHeight="1">
+    <row r="68" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="93">
         <v>1.3278999999999999E-2</v>
       </c>
@@ -12458,7 +12827,7 @@
         <v>-4.8690000000000001E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:36" ht="15" customHeight="1">
+    <row r="69" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="93">
         <v>1.3868E-2</v>
       </c>
@@ -12568,7 +12937,7 @@
         <v>-5.3179999999999998E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:36" ht="15" customHeight="1">
+    <row r="70" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="93">
         <v>1.4029E-2</v>
       </c>
@@ -12678,7 +13047,7 @@
         <v>-5.8690000000000001E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:36" ht="15" customHeight="1">
+    <row r="71" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="93">
         <v>1.3613999999999999E-2</v>
       </c>
@@ -12788,7 +13157,7 @@
         <v>-6.1539999999999997E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:36" ht="15" customHeight="1">
+    <row r="72" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="93">
         <v>1.3942E-2</v>
       </c>
@@ -12898,7 +13267,7 @@
         <v>-6.4120000000000002E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:36" ht="15" customHeight="1">
+    <row r="73" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="93">
         <v>1.3676000000000001E-2</v>
       </c>
@@ -13008,7 +13377,7 @@
         <v>-6.5750000000000001E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:36" ht="15" customHeight="1">
+    <row r="74" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="93">
         <v>1.3243E-2</v>
       </c>
@@ -13118,7 +13487,7 @@
         <v>-6.3759999999999997E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:36" ht="15" customHeight="1">
+    <row r="75" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="93">
         <v>1.324E-2</v>
       </c>
@@ -13228,7 +13597,7 @@
         <v>-6.1650000000000003E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:36" ht="15" customHeight="1">
+    <row r="76" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="93">
         <v>1.2917E-2</v>
       </c>
@@ -13338,7 +13707,7 @@
         <v>-5.9849999999999999E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:36" ht="15" customHeight="1">
+    <row r="77" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="93">
         <v>1.0728E-2</v>
       </c>
@@ -13448,11 +13817,11 @@
         <v>-5.4469999999999996E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:36" ht="15" customHeight="1">
+    <row r="78" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="96"/>
       <c r="AJ78" s="96"/>
     </row>
-    <row r="79" spans="1:36" ht="15" customHeight="1">
+    <row r="79" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="96"/>
       <c r="AJ79" s="96"/>
     </row>
@@ -13472,9 +13841,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:36" ht="15" customHeight="1">
+    <row r="1" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="93">
         <v>-3.7426000000000001E-2</v>
       </c>
@@ -13584,7 +13953,7 @@
         <v>2.0455000000000001E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="15" customHeight="1">
+    <row r="2" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="93">
         <v>-2.8854999999999999E-2</v>
       </c>
@@ -13694,7 +14063,7 @@
         <v>1.7618000000000002E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="15" customHeight="1">
+    <row r="3" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="93">
         <v>-1.6777E-2</v>
       </c>
@@ -13804,7 +14173,7 @@
         <v>1.2865E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:36" ht="15" customHeight="1">
+    <row r="4" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="93">
         <v>-1.3431999999999999E-2</v>
       </c>
@@ -13914,7 +14283,7 @@
         <v>8.5830000000000004E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:36" ht="15" customHeight="1">
+    <row r="5" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="93">
         <v>-9.0860000000000003E-3</v>
       </c>
@@ -14024,7 +14393,7 @@
         <v>4.6259999999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:36" ht="15" customHeight="1">
+    <row r="6" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="93">
         <v>-3.0370000000000002E-3</v>
       </c>
@@ -14134,7 +14503,7 @@
         <v>1.6850000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:36" ht="15" customHeight="1">
+    <row r="7" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="93">
         <v>-8.6000000000000003E-5</v>
       </c>
@@ -14244,7 +14613,7 @@
         <v>-1.0900000000000001E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:36" ht="15" customHeight="1">
+    <row r="8" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="93">
         <v>7.1699999999999997E-4</v>
       </c>
@@ -14354,7 +14723,7 @@
         <v>-9.990000000000001E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:36" ht="15" customHeight="1">
+    <row r="9" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="93">
         <v>1.9419999999999999E-3</v>
       </c>
@@ -14464,7 +14833,7 @@
         <v>-6.2699999999999995E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:36" ht="15" customHeight="1">
+    <row r="10" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="93">
         <v>2.2409999999999999E-3</v>
       </c>
@@ -14574,7 +14943,7 @@
         <v>-7.4799999999999997E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:36" ht="15" customHeight="1">
+    <row r="11" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="93">
         <v>1.7359999999999999E-3</v>
       </c>
@@ -14684,7 +15053,7 @@
         <v>-2.8400000000000002E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:36" ht="15" customHeight="1">
+    <row r="12" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="93">
         <v>2.7469999999999999E-3</v>
       </c>
@@ -14794,7 +15163,7 @@
         <v>1.6100000000000001E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:36" ht="15" customHeight="1">
+    <row r="13" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="93">
         <v>3.029E-3</v>
       </c>
@@ -14904,7 +15273,7 @@
         <v>2.6499999999999999E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:36" ht="15" customHeight="1">
+    <row r="14" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="93">
         <v>2.8159999999999999E-3</v>
       </c>
@@ -15014,7 +15383,7 @@
         <v>6.7599999999999995E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:36" ht="15" customHeight="1">
+    <row r="15" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="93">
         <v>3.1089999999999998E-3</v>
       </c>
@@ -15124,7 +15493,7 @@
         <v>8.4000000000000003E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:36" ht="15" customHeight="1">
+    <row r="16" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="93">
         <v>2.4489999999999998E-3</v>
       </c>
@@ -15234,7 +15603,7 @@
         <v>8.9899999999999995E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:36" ht="15" customHeight="1">
+    <row r="17" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="93">
         <v>3.4160000000000002E-3</v>
       </c>
@@ -15344,7 +15713,7 @@
         <v>7.4200000000000004E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:36" ht="15" customHeight="1">
+    <row r="18" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="93">
         <v>3.346E-3</v>
       </c>
@@ -15454,7 +15823,7 @@
         <v>7.6099999999999996E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:36" ht="15" customHeight="1">
+    <row r="19" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="93">
         <v>2.9710000000000001E-3</v>
       </c>
@@ -15564,7 +15933,7 @@
         <v>6.8400000000000004E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:36" ht="15" customHeight="1">
+    <row r="20" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="93">
         <v>3.604E-3</v>
       </c>
@@ -15674,7 +16043,7 @@
         <v>6.3900000000000003E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:36" ht="15" customHeight="1">
+    <row r="21" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="93">
         <v>3.3969999999999998E-3</v>
       </c>
@@ -15784,7 +16153,7 @@
         <v>6.1300000000000005E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:36" ht="15" customHeight="1">
+    <row r="22" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="93">
         <v>2.7720000000000002E-3</v>
       </c>
@@ -15894,7 +16263,7 @@
         <v>4.8899999999999996E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:36" ht="15" customHeight="1">
+    <row r="23" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="93">
         <v>2.9299999999999999E-3</v>
       </c>
@@ -16004,7 +16373,7 @@
         <v>4.9799999999999996E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:36" ht="15" customHeight="1">
+    <row r="24" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="93">
         <v>2.784E-3</v>
       </c>
@@ -16114,7 +16483,7 @@
         <v>4.3899999999999999E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:36" ht="15" customHeight="1">
+    <row r="25" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="93">
         <v>2.5490000000000001E-3</v>
       </c>
@@ -16224,7 +16593,7 @@
         <v>3.6499999999999998E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:36" ht="15" customHeight="1">
+    <row r="26" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="93">
         <v>3.0720000000000001E-3</v>
       </c>
@@ -16334,7 +16703,7 @@
         <v>1.5699999999999999E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:36" ht="15" customHeight="1">
+    <row r="27" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="93">
         <v>3.0149999999999999E-3</v>
       </c>
@@ -16444,7 +16813,7 @@
         <v>9.3999999999999994E-5</v>
       </c>
     </row>
-    <row r="28" spans="1:36" ht="15" customHeight="1">
+    <row r="28" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="93">
         <v>2.4580000000000001E-3</v>
       </c>
@@ -16554,7 +16923,7 @@
         <v>2.42E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:36" ht="15" customHeight="1">
+    <row r="29" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="93">
         <v>2.875E-3</v>
       </c>
@@ -16664,7 +17033,7 @@
         <v>4.1999999999999998E-5</v>
       </c>
     </row>
-    <row r="30" spans="1:36" ht="15" customHeight="1">
+    <row r="30" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="93">
         <v>2.7690000000000002E-3</v>
       </c>
@@ -16774,7 +17143,7 @@
         <v>-4.8000000000000001E-5</v>
       </c>
     </row>
-    <row r="31" spans="1:36" ht="15" customHeight="1">
+    <row r="31" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="93">
         <v>2.993E-3</v>
       </c>
@@ -16884,7 +17253,7 @@
         <v>-6.7000000000000002E-5</v>
       </c>
     </row>
-    <row r="32" spans="1:36" ht="15" customHeight="1">
+    <row r="32" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="93">
         <v>2.6129999999999999E-3</v>
       </c>
@@ -16994,7 +17363,7 @@
         <v>-1.11E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:36" ht="15" customHeight="1">
+    <row r="33" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="93">
         <v>2.722E-3</v>
       </c>
@@ -17104,7 +17473,7 @@
         <v>-5.1E-5</v>
       </c>
     </row>
-    <row r="34" spans="1:36" ht="15" customHeight="1">
+    <row r="34" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="93">
         <v>2.944E-3</v>
       </c>
@@ -17214,7 +17583,7 @@
         <v>-1.74E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:36" ht="15" customHeight="1">
+    <row r="35" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="93">
         <v>3.1470000000000001E-3</v>
       </c>
@@ -17324,7 +17693,7 @@
         <v>-2.0900000000000001E-4</v>
       </c>
     </row>
-    <row r="36" spans="1:36" ht="15" customHeight="1">
+    <row r="36" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="93">
         <v>3.3219999999999999E-3</v>
       </c>
@@ -17434,7 +17803,7 @@
         <v>-3.3E-4</v>
       </c>
     </row>
-    <row r="37" spans="1:36" ht="15" customHeight="1">
+    <row r="37" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="93">
         <v>3.1719999999999999E-3</v>
       </c>
@@ -17544,7 +17913,7 @@
         <v>-2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:36" ht="15" customHeight="1">
+    <row r="38" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="93">
         <v>2.9269999999999999E-3</v>
       </c>
@@ -17654,7 +18023,7 @@
         <v>-2.7799999999999998E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:36" ht="15" customHeight="1">
+    <row r="39" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="93">
         <v>2.8470000000000001E-3</v>
       </c>
@@ -17764,7 +18133,7 @@
         <v>-3.2600000000000001E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:36" ht="15" customHeight="1">
+    <row r="40" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="93">
         <v>2.9489999999999998E-3</v>
       </c>
@@ -17874,7 +18243,7 @@
         <v>-3.2600000000000001E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:36" ht="15" customHeight="1">
+    <row r="41" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="93">
         <v>2.6800000000000001E-3</v>
       </c>
@@ -17984,7 +18353,7 @@
         <v>-4.2400000000000001E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:36" ht="15" customHeight="1">
+    <row r="42" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="93">
         <v>2.6020000000000001E-3</v>
       </c>
@@ -18094,7 +18463,7 @@
         <v>-4.3899999999999999E-4</v>
       </c>
     </row>
-    <row r="43" spans="1:36" ht="15" customHeight="1">
+    <row r="43" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="93">
         <v>1.9750000000000002E-3</v>
       </c>
@@ -18204,7 +18573,7 @@
         <v>-1.7100000000000001E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:36" ht="15" customHeight="1">
+    <row r="44" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="93">
         <v>2.0240000000000002E-3</v>
       </c>
@@ -18314,7 +18683,7 @@
         <v>-1.6100000000000001E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:36" ht="15" customHeight="1">
+    <row r="45" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="93">
         <v>1.8209999999999999E-3</v>
       </c>
@@ -18424,7 +18793,7 @@
         <v>-2.5900000000000001E-4</v>
       </c>
     </row>
-    <row r="46" spans="1:36" ht="15" customHeight="1">
+    <row r="46" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="93">
         <v>1.737E-3</v>
       </c>
@@ -18534,7 +18903,7 @@
         <v>-3.4600000000000001E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:36" ht="15" customHeight="1">
+    <row r="47" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="93">
         <v>1.6819999999999999E-3</v>
       </c>
@@ -18644,7 +19013,7 @@
         <v>-3.4600000000000001E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:36" ht="15" customHeight="1">
+    <row r="48" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="93">
         <v>1.5560000000000001E-3</v>
       </c>
@@ -18754,7 +19123,7 @@
         <v>-1.7799999999999999E-4</v>
       </c>
     </row>
-    <row r="49" spans="1:36" ht="15" customHeight="1">
+    <row r="49" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="93">
         <v>1.815E-3</v>
       </c>
@@ -18864,7 +19233,7 @@
         <v>-3.1599999999999998E-4</v>
       </c>
     </row>
-    <row r="50" spans="1:36" ht="15" customHeight="1">
+    <row r="50" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="93">
         <v>1.9250000000000001E-3</v>
       </c>
@@ -18974,7 +19343,7 @@
         <v>-6.2200000000000005E-4</v>
       </c>
     </row>
-    <row r="51" spans="1:36" ht="15" customHeight="1">
+    <row r="51" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="93">
         <v>1.5E-3</v>
       </c>
@@ -19084,7 +19453,7 @@
         <v>-5.9800000000000001E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:36" ht="15" customHeight="1">
+    <row r="52" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="93">
         <v>1.487E-3</v>
       </c>
@@ -19194,7 +19563,7 @@
         <v>-5.4900000000000001E-4</v>
       </c>
     </row>
-    <row r="53" spans="1:36" ht="15" customHeight="1">
+    <row r="53" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="93">
         <v>1.4369999999999999E-3</v>
       </c>
@@ -19304,7 +19673,7 @@
         <v>-5.2700000000000002E-4</v>
       </c>
     </row>
-    <row r="54" spans="1:36" ht="15" customHeight="1">
+    <row r="54" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="93">
         <v>1.403E-3</v>
       </c>
@@ -19414,7 +19783,7 @@
         <v>-4.0200000000000001E-4</v>
       </c>
     </row>
-    <row r="55" spans="1:36" ht="15" customHeight="1">
+    <row r="55" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="93">
         <v>1.2949999999999999E-3</v>
       </c>
@@ -19524,7 +19893,7 @@
         <v>-3.6699999999999998E-4</v>
       </c>
     </row>
-    <row r="56" spans="1:36" ht="15" customHeight="1">
+    <row r="56" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="93">
         <v>1.1590000000000001E-3</v>
       </c>
@@ -19634,7 +20003,7 @@
         <v>-3.9500000000000001E-4</v>
       </c>
     </row>
-    <row r="57" spans="1:36" ht="15" customHeight="1">
+    <row r="57" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="93">
         <v>1.1640000000000001E-3</v>
       </c>
@@ -19744,7 +20113,7 @@
         <v>-2.7099999999999997E-4</v>
       </c>
     </row>
-    <row r="58" spans="1:36" ht="15" customHeight="1">
+    <row r="58" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="93">
         <v>1.2440000000000001E-3</v>
       </c>
@@ -19854,7 +20223,7 @@
         <v>-1.9000000000000001E-4</v>
       </c>
     </row>
-    <row r="59" spans="1:36" ht="15" customHeight="1">
+    <row r="59" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="93">
         <v>1.096E-3</v>
       </c>
@@ -19964,7 +20333,7 @@
         <v>-1.5999999999999999E-5</v>
       </c>
     </row>
-    <row r="60" spans="1:36" ht="15" customHeight="1">
+    <row r="60" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="93">
         <v>1.114E-3</v>
       </c>
@@ -20074,7 +20443,7 @@
         <v>6.8999999999999997E-5</v>
       </c>
     </row>
-    <row r="61" spans="1:36" ht="15" customHeight="1">
+    <row r="61" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="93">
         <v>1.222E-3</v>
       </c>
@@ -20184,7 +20553,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="62" spans="1:36" ht="15" customHeight="1">
+    <row r="62" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="93">
         <v>1.0989999999999999E-3</v>
       </c>
@@ -20294,7 +20663,7 @@
         <v>3.7100000000000002E-4</v>
       </c>
     </row>
-    <row r="63" spans="1:36" ht="15" customHeight="1">
+    <row r="63" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="93">
         <v>1.067E-3</v>
       </c>
@@ -20404,7 +20773,7 @@
         <v>6.4000000000000005E-4</v>
       </c>
     </row>
-    <row r="64" spans="1:36" ht="15" customHeight="1">
+    <row r="64" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="93">
         <v>1.1640000000000001E-3</v>
       </c>
@@ -20514,7 +20883,7 @@
         <v>8.3100000000000003E-4</v>
       </c>
     </row>
-    <row r="65" spans="1:36" ht="15" customHeight="1">
+    <row r="65" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="93">
         <v>1.0430000000000001E-3</v>
       </c>
@@ -20624,7 +20993,7 @@
         <v>8.7799999999999998E-4</v>
       </c>
     </row>
-    <row r="66" spans="1:36" ht="15" customHeight="1">
+    <row r="66" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="93">
         <v>1.0529999999999999E-3</v>
       </c>
@@ -20734,7 +21103,7 @@
         <v>1.0219999999999999E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:36" ht="15" customHeight="1">
+    <row r="67" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="93">
         <v>9.3599999999999998E-4</v>
       </c>
@@ -20844,7 +21213,7 @@
         <v>1.1299999999999999E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:36" ht="15" customHeight="1">
+    <row r="68" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="93">
         <v>7.6000000000000004E-4</v>
       </c>
@@ -20954,7 +21323,7 @@
         <v>1.191E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:36" ht="15" customHeight="1">
+    <row r="69" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="93">
         <v>7.7099999999999998E-4</v>
       </c>
@@ -21064,7 +21433,7 @@
         <v>1.042E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:36" ht="15" customHeight="1">
+    <row r="70" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="93">
         <v>9.1200000000000005E-4</v>
       </c>
@@ -21174,7 +21543,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
     </row>
-    <row r="71" spans="1:36" ht="15" customHeight="1">
+    <row r="71" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="93">
         <v>9.2699999999999998E-4</v>
       </c>
@@ -21284,7 +21653,7 @@
         <v>6.0700000000000001E-4</v>
       </c>
     </row>
-    <row r="72" spans="1:36" ht="15" customHeight="1">
+    <row r="72" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="93">
         <v>1.127E-3</v>
       </c>
@@ -21394,7 +21763,7 @@
         <v>4.3600000000000003E-4</v>
       </c>
     </row>
-    <row r="73" spans="1:36" ht="15" customHeight="1">
+    <row r="73" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="93">
         <v>1.049E-3</v>
       </c>
@@ -21504,7 +21873,7 @@
         <v>2.0799999999999999E-4</v>
       </c>
     </row>
-    <row r="74" spans="1:36" ht="15" customHeight="1">
+    <row r="74" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="93">
         <v>9.6400000000000001E-4</v>
       </c>
@@ -21614,7 +21983,7 @@
         <v>1.64E-4</v>
       </c>
     </row>
-    <row r="75" spans="1:36" ht="15" customHeight="1">
+    <row r="75" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="93">
         <v>8.9599999999999999E-4</v>
       </c>
@@ -21724,7 +22093,7 @@
         <v>1.92E-4</v>
       </c>
     </row>
-    <row r="76" spans="1:36" ht="15" customHeight="1">
+    <row r="76" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="93">
         <v>4.4700000000000002E-4</v>
       </c>
@@ -21834,7 +22203,7 @@
         <v>2.9100000000000003E-4</v>
       </c>
     </row>
-    <row r="77" spans="1:36" ht="15" customHeight="1">
+    <row r="77" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="93">
         <v>-1.8000000000000001E-4</v>
       </c>

</xml_diff>